<commit_message>
Fixed some mistakes in the Memory unit
</commit_message>
<xml_diff>
--- a/RISC-V-Instructions.xlsx
+++ b/RISC-V-Instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\disho\Documents\GitHub\cpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C7B745-A9C0-432F-A2AB-F01B3C17DC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DD3E2C-0CAA-427F-A022-C856FDD8E2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6450" yWindow="5640" windowWidth="21600" windowHeight="11295" xr2:uid="{3A4DAA86-2582-41E6-9E68-1394027EFF25}"/>
+    <workbookView xWindow="6450" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{3A4DAA86-2582-41E6-9E68-1394027EFF25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -864,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE828DAB-632D-493B-A748-1CC9E671C85A}">
   <dimension ref="A1:AG1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q20" zoomScale="76" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE39" sqref="AE39"/>
+    <sheetView tabSelected="1" topLeftCell="P16" zoomScale="76" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG24" sqref="AG24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>